<commit_message>
add requirement.txt for installing python libraries
</commit_message>
<xml_diff>
--- a/stock_manager/example.xlsx
+++ b/stock_manager/example.xlsx
@@ -5,17 +5,17 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jwahn37/Dropbox/제테크/money_maker/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jwahn37/Dropbox/제테크/money_maker/stock_manager/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{600CDC9E-B375-BC40-A624-93379241E4BC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4C879FE9-46EC-D743-8909-9B527F73144A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16000" xr2:uid="{CC71CE27-A0D1-F14E-AC6F-1406CBD18417}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="25600" windowHeight="14020" xr2:uid="{CC71CE27-A0D1-F14E-AC6F-1406CBD18417}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -721,8 +721,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{53774EF4-537C-5649-886A-6DA812206DCA}">
   <dimension ref="A1:D36"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A18" sqref="A18"/>
+    <sheetView tabSelected="1" topLeftCell="A11" workbookViewId="0">
+      <selection activeCell="A26" sqref="A26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="18"/>
@@ -747,10 +747,10 @@
         <v>1</v>
       </c>
       <c r="B2" s="7">
-        <v>71336.649999999994</v>
+        <v>71429.02</v>
       </c>
       <c r="D2" s="11">
-        <v>1197.2</v>
+        <v>1197.5</v>
       </c>
     </row>
     <row r="3" spans="1:4">
@@ -774,7 +774,7 @@
         <v>4</v>
       </c>
       <c r="B5" s="7">
-        <v>74600</v>
+        <v>74800</v>
       </c>
     </row>
     <row r="6" spans="1:4">
@@ -782,7 +782,7 @@
         <v>5</v>
       </c>
       <c r="B6" s="7">
-        <v>316500</v>
+        <v>317000</v>
       </c>
     </row>
     <row r="7" spans="1:4">
@@ -798,7 +798,7 @@
         <v>7</v>
       </c>
       <c r="B8" s="7">
-        <v>79800</v>
+        <v>79900</v>
       </c>
     </row>
     <row r="9" spans="1:4">
@@ -806,7 +806,7 @@
         <v>8</v>
       </c>
       <c r="B9" s="7">
-        <v>123500</v>
+        <v>123000</v>
       </c>
     </row>
     <row r="10" spans="1:4">
@@ -814,7 +814,7 @@
         <v>9</v>
       </c>
       <c r="B10" s="7">
-        <v>78600</v>
+        <v>78300</v>
       </c>
     </row>
     <row r="11" spans="1:4">
@@ -822,7 +822,7 @@
         <v>10</v>
       </c>
       <c r="B11" s="7">
-        <v>8175</v>
+        <v>8165</v>
       </c>
     </row>
     <row r="12" spans="1:4">
@@ -830,7 +830,7 @@
         <v>11</v>
       </c>
       <c r="B12" s="7">
-        <v>18630</v>
+        <v>18600</v>
       </c>
     </row>
     <row r="13" spans="1:4">
@@ -838,7 +838,7 @@
         <v>12</v>
       </c>
       <c r="B13" s="7">
-        <v>11420</v>
+        <v>11435</v>
       </c>
     </row>
     <row r="14" spans="1:4">
@@ -846,7 +846,7 @@
         <v>13</v>
       </c>
       <c r="B14" s="7">
-        <v>28625</v>
+        <v>28630</v>
       </c>
     </row>
     <row r="15" spans="1:4">
@@ -854,7 +854,7 @@
         <v>14</v>
       </c>
       <c r="B15" s="7">
-        <v>23505</v>
+        <v>23385</v>
       </c>
     </row>
     <row r="16" spans="1:4">
@@ -870,7 +870,7 @@
         <v>16</v>
       </c>
       <c r="B17" s="7">
-        <v>5960</v>
+        <v>5965</v>
       </c>
     </row>
     <row r="18" spans="1:2">
@@ -886,7 +886,7 @@
         <v>18</v>
       </c>
       <c r="B19" s="7">
-        <v>13430</v>
+        <v>13445</v>
       </c>
     </row>
     <row r="20" spans="1:2">
@@ -894,7 +894,7 @@
         <v>37</v>
       </c>
       <c r="B20" s="7">
-        <v>15340</v>
+        <v>15270</v>
       </c>
     </row>
     <row r="21" spans="1:2">
@@ -902,7 +902,7 @@
         <v>19</v>
       </c>
       <c r="B21" s="7">
-        <v>449500</v>
+        <v>455500</v>
       </c>
     </row>
     <row r="22" spans="1:2">
@@ -910,7 +910,7 @@
         <v>20</v>
       </c>
       <c r="B22" s="7">
-        <v>54300</v>
+        <v>54700</v>
       </c>
     </row>
     <row r="23" spans="1:2">
@@ -990,7 +990,7 @@
         <v>30</v>
       </c>
       <c r="B32" s="7">
-        <v>53435000</v>
+        <v>53379000</v>
       </c>
     </row>
     <row r="33" spans="1:2">
@@ -998,7 +998,7 @@
         <v>31</v>
       </c>
       <c r="B33" s="7">
-        <v>3792000</v>
+        <v>3791000</v>
       </c>
     </row>
     <row r="34" spans="1:2">
@@ -1006,7 +1006,7 @@
         <v>32</v>
       </c>
       <c r="B34" s="10">
-        <v>2.11160960618807</v>
+        <v>2.1310345312666299</v>
       </c>
     </row>
     <row r="35" spans="1:2">

</xml_diff>